<commit_message>
- Implemented filtering and pagination in Institutional Prices Tab - Implemented Statistics page
Started work on Institution Filter on Pricing tab

Implemented jQuery DataTables to filter Institutions of Prices page

Fixed domain regex matching

Changed column names for License import files

Domain -> Domains
ISSN -> eISSN

Started implementing statistics page

Implemented Statistics page

Removed unnecessary comments

Fixed Issue with duplicate domains

Included DataTables as a local bundle

Added non-minified datatables scripts.

Also, Removed JournalsController.js source maps because they where not
being refreshed

disabled bundling

Removed unnecessary form
</commit_message>
<xml_diff>
--- a/tests/Core.Tests/Import/SubmissionLinks/Stubs/Submission-links.xlsx
+++ b/tests/Core.Tests/Import/SubmissionLinks/Stubs/Submission-links.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>eissn</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>http://campus.usal.es/~revistas_trabajo/index.php/1130-2887/submission</t>
+  </si>
+  <si>
+    <t>2076-3387</t>
+  </si>
+  <si>
+    <t>http://susy.mdpi.com</t>
   </si>
 </sst>
 </file>
@@ -421,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,41 +453,49 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -490,13 +504,14 @@
     <sortCondition ref="C1"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>